<commit_message>
Update tab switching with tab cache
</commit_message>
<xml_diff>
--- a/backend/Templates/CB_for_staff_Export_Template.xlsx
+++ b/backend/Templates/CB_for_staff_Export_Template.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Software_Development_Project\AFN-II_Database_Web_Application\backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Software_Development_Project\AFN-II_Database_Web_Application\backend\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648BAF33-E8D2-4D7C-8AC5-B0537C5E6FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51CDF514-3665-471E-B2F1-FDFB1365C4F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$6:$T$6</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t xml:space="preserve">C1,2,3 </t>
   </si>
@@ -79,9 +82,6 @@
  (AFN-II staff, GoL staff, WFP staff )</t>
   </si>
   <si>
-    <t>Gender</t>
-  </si>
-  <si>
     <t>Training Type
 (1-ToT, 2-Traning, 3-Study visit, 4-On-the-job training, 5-on-site demonstrations,6-Meeting)</t>
   </si>
@@ -123,7 +123,14 @@
 Complete</t>
   </si>
   <si>
-    <t>SID</t>
+    <t>ອາຍຸ (Age)</t>
+  </si>
+  <si>
+    <t>ເພດ (ຍິງ/ຊາຍ)
+(M/F)</t>
+  </si>
+  <si>
+    <t>SubmissionID</t>
   </si>
 </sst>
 </file>
@@ -401,7 +408,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -442,26 +449,6 @@
     </xf>
     <xf numFmtId="14" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -498,10 +485,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="164" fontId="9" fillId="3" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -518,6 +501,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -525,6 +512,28 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -809,188 +818,196 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="3.85546875" style="10" customWidth="1"/>
-    <col min="2" max="2" width="3.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="10" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="10" customWidth="1"/>
     <col min="4" max="4" width="21" style="10" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="12" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" style="12" customWidth="1"/>
-    <col min="7" max="7" width="24.5703125" style="10" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" style="10" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" style="10" customWidth="1"/>
-    <col min="10" max="10" width="21" style="10" customWidth="1"/>
-    <col min="11" max="11" width="21.5703125" style="10" customWidth="1"/>
-    <col min="12" max="12" width="21.140625" style="10" customWidth="1"/>
-    <col min="13" max="13" width="37.7109375" style="10" customWidth="1"/>
-    <col min="14" max="14" width="30.42578125" style="10" customWidth="1"/>
-    <col min="15" max="15" width="20.140625" style="13" customWidth="1"/>
-    <col min="16" max="16" width="19.28515625" style="13" customWidth="1"/>
-    <col min="17" max="17" width="17.42578125" style="13" customWidth="1"/>
-    <col min="18" max="18" width="18.42578125" style="13" customWidth="1"/>
-    <col min="19" max="19" width="19.28515625" style="13" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="10"/>
+    <col min="5" max="5" width="18.42578125" style="12" customWidth="1"/>
+    <col min="6" max="6" width="20" style="12" customWidth="1"/>
+    <col min="7" max="7" width="31.28515625" style="10" customWidth="1"/>
+    <col min="8" max="8" width="7.28515625" style="10" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" style="10" customWidth="1"/>
+    <col min="10" max="10" width="28.5703125" style="10" customWidth="1"/>
+    <col min="11" max="11" width="33.28515625" style="10" customWidth="1"/>
+    <col min="12" max="12" width="21" style="10" customWidth="1"/>
+    <col min="13" max="13" width="24.28515625" style="10" customWidth="1"/>
+    <col min="14" max="14" width="58.5703125" style="10" customWidth="1"/>
+    <col min="15" max="15" width="30.42578125" style="10" customWidth="1"/>
+    <col min="16" max="16" width="27.140625" style="13" customWidth="1"/>
+    <col min="17" max="17" width="25" style="13" customWidth="1"/>
+    <col min="18" max="18" width="24.85546875" style="13" customWidth="1"/>
+    <col min="19" max="19" width="23.5703125" style="13" customWidth="1"/>
+    <col min="20" max="20" width="27.42578125" style="13" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:20" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
+      <c r="B1" s="15"/>
       <c r="C1" s="9"/>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="2"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="1"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
     </row>
-    <row r="2" spans="1:19" ht="18" x14ac:dyDescent="0.35">
-      <c r="A2" s="21"/>
-      <c r="B2" s="22"/>
+    <row r="2" spans="1:20" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="16"/>
+      <c r="B2" s="17"/>
       <c r="C2" s="9"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="2"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="1"/>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="24"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="Q3" s="25"/>
+      <c r="R3" s="25"/>
+      <c r="S3" s="25"/>
+      <c r="T3" s="25"/>
+    </row>
+    <row r="4" spans="1:20" ht="54" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="28"/>
+      <c r="G4" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="28" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="P3" s="31"/>
-      <c r="Q3" s="31"/>
-      <c r="R3" s="31"/>
-      <c r="S3" s="31"/>
+      <c r="J4" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="M4" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="N4" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="O4" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4" s="32" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q4" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="R4" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="S4" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="T4" s="32" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="34"/>
-      <c r="G4" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="K4" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="L4" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="M4" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="N4" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="O4" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="P4" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q4" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="R4" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="S4" s="17" t="s">
+    <row r="5" spans="1:20" ht="41.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="6"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="27"/>
+      <c r="D5" s="27"/>
+      <c r="E5" s="11" t="s">
         <v>19</v>
       </c>
+      <c r="F5" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="29"/>
+      <c r="H5" s="37"/>
+      <c r="I5" s="37"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="35"/>
+      <c r="P5" s="33"/>
+      <c r="Q5" s="33"/>
+      <c r="R5" s="33"/>
+      <c r="S5" s="33"/>
+      <c r="T5" s="33"/>
     </row>
-    <row r="5" spans="1:19" ht="28.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="6"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="16"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="16"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="18"/>
-      <c r="Q5" s="18"/>
-      <c r="R5" s="18"/>
-      <c r="S5" s="18"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
       <c r="B6" s="8">
         <v>1</v>
@@ -1046,30 +1063,35 @@
       <c r="S6" s="8">
         <v>18</v>
       </c>
+      <c r="T6" s="8">
+        <v>19</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <autoFilter ref="B6:T6" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <mergeCells count="22">
+    <mergeCell ref="H4:H5"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
     <mergeCell ref="A1:B2"/>
-    <mergeCell ref="D1:M2"/>
+    <mergeCell ref="D1:N2"/>
     <mergeCell ref="B3:B5"/>
-    <mergeCell ref="D3:K3"/>
-    <mergeCell ref="O3:S3"/>
+    <mergeCell ref="D3:L3"/>
+    <mergeCell ref="P3:T3"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="G4:G5"/>
-    <mergeCell ref="H4:H5"/>
-    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="J4:J5"/>
+    <mergeCell ref="K4:K5"/>
     <mergeCell ref="C3:C5"/>
-    <mergeCell ref="P4:P5"/>
     <mergeCell ref="Q4:Q5"/>
     <mergeCell ref="R4:R5"/>
     <mergeCell ref="S4:S5"/>
-    <mergeCell ref="J4:J5"/>
-    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="T4:T5"/>
     <mergeCell ref="L4:L5"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="O4:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>